<commit_message>
Changes on the header, login and reg functions
</commit_message>
<xml_diff>
--- a/AdsOnSPA/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/AdsOnSPA/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -841,7 +841,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
@@ -865,7 +865,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
@@ -912,7 +912,9 @@
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
@@ -946,7 +948,9 @@
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
       <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
@@ -956,7 +960,9 @@
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
@@ -966,7 +972,9 @@
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
@@ -976,7 +984,9 @@
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
@@ -986,7 +996,9 @@
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
@@ -996,7 +1008,9 @@
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1006,7 +1020,9 @@
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
@@ -1220,7 +1236,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Login and Logout finilized
</commit_message>
<xml_diff>
--- a/AdsOnSPA/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/AdsOnSPA/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -686,7 +686,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +913,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
@@ -1033,7 +1033,7 @@
         <v>23</v>
       </c>
       <c r="C31" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>5</v>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>